<commit_message>
TP1 Metricas con desarrollo
</commit_message>
<xml_diff>
--- a/TP1/Metricas.xlsx
+++ b/TP1/Metricas.xlsx
@@ -765,11 +765,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="6" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -780,61 +787,22 @@
     <xf numFmtId="49" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -845,16 +813,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -863,6 +821,48 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="6" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -989,7 +989,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Métricas!$B$28:$D$32</c:f>
+              <c:f>Métricas!$B$27:$D$31</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1012,7 +1012,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Métricas!$E$28:$E$32</c:f>
+              <c:f>Métricas!$E$27:$E$31</c:f>
               <c:numCache>
                 <c:formatCode>[h]:mm</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1026,10 +1026,10 @@
                   <c:v>5.2083333333333315E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2.7777777777777779E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>4.4444444444444509E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1085,13 +1085,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>9527</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1403,8 +1403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1422,29 +1422,29 @@
       <c r="B1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="63"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="57"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -1470,15 +1470,15 @@
       <c r="E3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="82"/>
-      <c r="N3" s="82"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="65"/>
       <c r="O3" s="14"/>
       <c r="P3" s="9"/>
     </row>
@@ -1497,15 +1497,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C4),ISBLANK(D4)),"Completar",IF(D4&gt;=C4,D4-C4,"Error")),"Error")</f>
         <v>3.4722222222222654E-3</v>
       </c>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="64"/>
-      <c r="N4" s="64"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="66"/>
       <c r="O4" s="15"/>
       <c r="P4" s="11"/>
     </row>
@@ -1529,12 +1529,12 @@
     </row>
     <row r="6" spans="1:16" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="63"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="57"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -1560,15 +1560,15 @@
       <c r="E7" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="82"/>
-      <c r="L7" s="82"/>
-      <c r="M7" s="82"/>
-      <c r="N7" s="82"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="65"/>
+      <c r="M7" s="65"/>
+      <c r="N7" s="65"/>
       <c r="O7" s="14"/>
       <c r="P7" s="9"/>
     </row>
@@ -1587,15 +1587,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C8),ISBLANK(D8)),"Completar",IF(D8&gt;=C8,D8-C8,"Error")),"Error")</f>
         <v>4.7916666666666607E-2</v>
       </c>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="64"/>
-      <c r="K8" s="64"/>
-      <c r="L8" s="64"/>
-      <c r="M8" s="64"/>
-      <c r="N8" s="64"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
+      <c r="I8" s="66"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="66"/>
+      <c r="L8" s="66"/>
+      <c r="M8" s="66"/>
+      <c r="N8" s="66"/>
       <c r="O8" s="15"/>
       <c r="P8" s="11"/>
     </row>
@@ -1619,50 +1619,50 @@
     </row>
     <row r="10" spans="1:16" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="62"/>
-      <c r="N10" s="63"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="57"/>
       <c r="O10" s="13"/>
     </row>
     <row r="11" spans="1:16" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="74"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="76" t="s">
+      <c r="D11" s="72"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="77"/>
-      <c r="H11" s="73" t="s">
+      <c r="G11" s="62"/>
+      <c r="H11" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="74"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="76" t="s">
+      <c r="I11" s="72"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="L11" s="77"/>
-      <c r="M11" s="73" t="s">
+      <c r="L11" s="62"/>
+      <c r="M11" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="81" t="s">
+      <c r="N11" s="64" t="s">
         <v>2</v>
       </c>
       <c r="O11" s="14"/>
@@ -1670,10 +1670,10 @@
     </row>
     <row r="12" spans="1:16" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
-      <c r="B12" s="65"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="75"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="73"/>
       <c r="F12" s="18" t="s">
         <v>13</v>
       </c>
@@ -1695,8 +1695,8 @@
       <c r="L12" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="M12" s="73"/>
-      <c r="N12" s="81"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="64"/>
       <c r="O12" s="14"/>
       <c r="P12" s="9"/>
     </row>
@@ -1706,29 +1706,39 @@
         <f>ROW($B13)-12</f>
         <v>1</v>
       </c>
-      <c r="C13" s="78" t="s">
+      <c r="C13" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="78"/>
-      <c r="E13" s="79"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="68"/>
       <c r="F13" s="47">
         <v>20</v>
       </c>
       <c r="G13" s="48">
         <v>2.7777777777777779E-3</v>
       </c>
-      <c r="H13" s="49"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="20" t="str">
+      <c r="H13" s="49">
+        <v>0.3125</v>
+      </c>
+      <c r="I13" s="50">
+        <v>0.31597222222222221</v>
+      </c>
+      <c r="J13" s="20">
         <f>IFERROR(IF(OR(ISBLANK(H13),ISBLANK(I13)),"Completar",IF(I13&gt;=H13,I13-H13,"Error")),"Error")</f>
-        <v>Completar</v>
-      </c>
-      <c r="K13" s="51"/>
-      <c r="L13" s="52"/>
-      <c r="M13" s="53"/>
-      <c r="N13" s="25" t="str">
+        <v>3.4722222222222099E-3</v>
+      </c>
+      <c r="K13" s="51">
+        <v>0</v>
+      </c>
+      <c r="L13" s="52">
+        <v>0</v>
+      </c>
+      <c r="M13" s="53">
+        <v>23</v>
+      </c>
+      <c r="N13" s="25">
         <f>IFERROR(IF(OR(J13="Completar",ISBLANK(L13)),"Completar",J13+L13),"Error")</f>
-        <v>Completar</v>
+        <v>3.4722222222222099E-3</v>
       </c>
       <c r="O13" s="15"/>
       <c r="P13" s="11"/>
@@ -1736,32 +1746,42 @@
     <row r="14" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="24">
-        <f t="shared" ref="B14:B16" si="0">ROW($B14)-12</f>
+        <f t="shared" ref="B14:B15" si="0">ROW($B14)-12</f>
         <v>2</v>
       </c>
-      <c r="C14" s="78" t="s">
+      <c r="C14" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="78"/>
-      <c r="E14" s="79"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="68"/>
       <c r="F14" s="47">
         <v>20</v>
       </c>
       <c r="G14" s="48">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="H14" s="49"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="20" t="str">
-        <f t="shared" ref="J14:J16" si="1">IFERROR(IF(OR(ISBLANK(H14),ISBLANK(I14)),"Completar",IF(I14&gt;=H14,I14-H14,"Error")),"Error")</f>
-        <v>Completar</v>
-      </c>
-      <c r="K14" s="51"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="53"/>
-      <c r="N14" s="25" t="str">
-        <f t="shared" ref="N14:N16" si="2">IFERROR(IF(OR(J14="Completar",ISBLANK(L14)),"Completar",J14+L14),"Error")</f>
-        <v>Completar</v>
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="H14" s="49">
+        <v>0.31666666666666665</v>
+      </c>
+      <c r="I14" s="50">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="J14" s="20">
+        <f t="shared" ref="J14:J15" si="1">IFERROR(IF(OR(ISBLANK(H14),ISBLANK(I14)),"Completar",IF(I14&gt;=H14,I14-H14,"Error")),"Error")</f>
+        <v>3.0555555555555614E-2</v>
+      </c>
+      <c r="K14" s="51">
+        <v>2</v>
+      </c>
+      <c r="L14" s="52">
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="M14" s="53">
+        <v>34</v>
+      </c>
+      <c r="N14" s="25">
+        <f t="shared" ref="N14:N15" si="2">IFERROR(IF(OR(J14="Completar",ISBLANK(L14)),"Completar",J14+L14),"Error")</f>
+        <v>3.3333333333333388E-2</v>
       </c>
       <c r="O14" s="15"/>
       <c r="P14" s="11"/>
@@ -1772,255 +1792,258 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C15" s="78" t="s">
+      <c r="C15" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="78"/>
-      <c r="E15" s="79"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="68"/>
       <c r="F15" s="47">
         <v>20</v>
       </c>
       <c r="G15" s="48">
-        <v>2.7777777777777779E-3</v>
-      </c>
-      <c r="H15" s="49"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="20" t="str">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="H15" s="49">
+        <v>0.34791666666666665</v>
+      </c>
+      <c r="I15" s="50">
+        <v>0.35833333333333334</v>
+      </c>
+      <c r="J15" s="20">
         <f t="shared" si="1"/>
-        <v>Completar</v>
-      </c>
-      <c r="K15" s="51"/>
-      <c r="L15" s="52"/>
-      <c r="M15" s="53"/>
-      <c r="N15" s="25" t="str">
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="K15" s="51">
+        <v>0</v>
+      </c>
+      <c r="L15" s="52">
+        <v>0</v>
+      </c>
+      <c r="M15" s="53">
+        <v>24</v>
+      </c>
+      <c r="N15" s="25">
         <f t="shared" si="2"/>
-        <v>Completar</v>
+        <v>1.0416666666666685E-2</v>
       </c>
       <c r="O15" s="15"/>
       <c r="P15" s="11"/>
     </row>
-    <row r="16" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="24">
-        <f t="shared" si="0"/>
+    <row r="16" spans="1:16" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="14"/>
+      <c r="B16" s="69" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="71"/>
+      <c r="F16" s="26">
+        <f>SUM(F13:F15)</f>
+        <v>60</v>
+      </c>
+      <c r="G16" s="27">
+        <f>SUM(G13:G15)</f>
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="H16" s="28"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="30">
+        <f>IF(OR(COUNTIF(J13:J15,"Error")&gt;0,COUNTIF(J13:J15,"Completar")&gt;0),"Error",SUM(J13:J15))</f>
+        <v>4.4444444444444509E-2</v>
+      </c>
+      <c r="K16" s="31">
+        <f>SUM(K13:K15)</f>
+        <v>2</v>
+      </c>
+      <c r="L16" s="27">
+        <f>SUM(L13:L15)</f>
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="M16" s="32">
+        <f>SUM(M13:M15)</f>
+        <v>81</v>
+      </c>
+      <c r="N16" s="33">
+        <f>IF(OR(COUNTIF(N13:N15,"Error")&gt;0,COUNTIF(N13:N15,"Completar")&gt;0),"Error",SUM(N13:N15))</f>
+        <v>4.7222222222222283E-2</v>
+      </c>
+      <c r="O16" s="14"/>
+      <c r="P16" s="17"/>
+    </row>
+    <row r="17" spans="1:16" s="7" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="16"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+    </row>
+    <row r="18" spans="1:16" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="13"/>
+    </row>
+    <row r="19" spans="1:16" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="79"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v>Completar</v>
-      </c>
-      <c r="K16" s="51"/>
-      <c r="L16" s="52"/>
-      <c r="M16" s="53"/>
-      <c r="N16" s="25" t="str">
-        <f t="shared" si="2"/>
-        <v>Completar</v>
-      </c>
-      <c r="O16" s="15"/>
-      <c r="P16" s="11"/>
-    </row>
-    <row r="17" spans="1:16" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
-      <c r="B17" s="83" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="84"/>
-      <c r="D17" s="84"/>
-      <c r="E17" s="85"/>
-      <c r="F17" s="26">
-        <f>SUM(F13:F16)</f>
-        <v>60</v>
-      </c>
-      <c r="G17" s="27">
-        <f>SUM(G13:G16)</f>
-        <v>1.9444444444444445E-2</v>
-      </c>
-      <c r="H17" s="28"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="30" t="str">
-        <f>IF(OR(COUNTIF(J13:J16,"Error")&gt;0,COUNTIF(J13:J16,"Completar")&gt;0),"Error",SUM(J13:J16))</f>
-        <v>Error</v>
-      </c>
-      <c r="K17" s="31">
-        <f>SUM(K13:K16)</f>
-        <v>0</v>
-      </c>
-      <c r="L17" s="27">
-        <f>SUM(L13:L16)</f>
-        <v>0</v>
-      </c>
-      <c r="M17" s="32">
-        <f>SUM(M13:M16)</f>
-        <v>0</v>
-      </c>
-      <c r="N17" s="33" t="str">
-        <f>IF(OR(COUNTIF(N13:N16,"Error")&gt;0,COUNTIF(N13:N16,"Completar")&gt;0),"Error",SUM(N13:N16))</f>
-        <v>Error</v>
-      </c>
-      <c r="O17" s="14"/>
-      <c r="P17" s="17"/>
-    </row>
-    <row r="18" spans="1:16" s="7" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="16"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
-    </row>
-    <row r="19" spans="1:16" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="61" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="63"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="13"/>
-    </row>
-    <row r="20" spans="1:16" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="5" t="s">
+      <c r="D19" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E19" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="9"/>
-    </row>
-    <row r="21" spans="1:16" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="15"/>
-      <c r="B21" s="45">
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="9"/>
+    </row>
+    <row r="20" spans="1:16" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="15"/>
+      <c r="B20" s="45">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="C21" s="46">
+      <c r="C20" s="46">
         <v>0.3125</v>
       </c>
-      <c r="D21" s="46">
+      <c r="D20" s="46">
         <v>0.36458333333333331</v>
       </c>
-      <c r="E21" s="33">
-        <f>IFERROR(IF(OR(ISBLANK(C21),ISBLANK(D21)),"Completar",IF(D21&gt;=C21,D21-C21,"Error")),"Error")</f>
+      <c r="E20" s="33">
+        <f>IFERROR(IF(OR(ISBLANK(C20),ISBLANK(D20)),"Completar",IF(D20&gt;=C20,D20-C20,"Error")),"Error")</f>
         <v>5.2083333333333315E-2</v>
       </c>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="11"/>
-    </row>
-    <row r="22" spans="1:16" s="7" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="16"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="16"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="16"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="61" t="s">
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="11"/>
+    </row>
+    <row r="21" spans="1:16" s="7" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B22" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="62"/>
-      <c r="L23" s="62"/>
-      <c r="M23" s="62"/>
-      <c r="N23" s="63"/>
-    </row>
-    <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="56" t="s">
+      <c r="C22" s="56"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="56"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="56"/>
+      <c r="L22" s="56"/>
+      <c r="M22" s="56"/>
+      <c r="N22" s="57"/>
+    </row>
+    <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="57"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="69">
-        <f>M17</f>
-        <v>0</v>
-      </c>
-      <c r="F24" s="70"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="35"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="35"/>
-      <c r="N24" s="38"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="56" t="s">
+      <c r="C23" s="59"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="82">
+        <f>M16</f>
+        <v>81</v>
+      </c>
+      <c r="F23" s="83"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="35"/>
+      <c r="L23" s="35"/>
+      <c r="M23" s="35"/>
+      <c r="N23" s="38"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B24" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="57"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="71">
-        <f>IF(M17=0,0,IFERROR(M17/(N17*24),"Error"))</f>
-        <v>0</v>
-      </c>
-      <c r="F25" s="72"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="84">
+        <f>IF(M16=0,0,IFERROR(M16/(N16*24),"Error"))</f>
+        <v>71.470588235294016</v>
+      </c>
+      <c r="F24" s="85"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="37"/>
+      <c r="N24" s="39"/>
+    </row>
+    <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="59"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="82">
+        <f>IF(K16=0,0,IFERROR(ROUNDUP(K16/(M16/100),0),"Error"))</f>
+        <v>3</v>
+      </c>
+      <c r="F25" s="83"/>
       <c r="G25" s="36"/>
       <c r="H25" s="37"/>
       <c r="I25" s="37"/>
@@ -2031,16 +2054,16 @@
       <c r="N25" s="39"/>
     </row>
     <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="56" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="57"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="69">
-        <f>IF(K17=0,0,IFERROR(ROUNDUP(K17/(M17/100),0),"Error"))</f>
-        <v>0</v>
-      </c>
-      <c r="F26" s="70"/>
+      <c r="B26" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="59"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="74">
+        <f>IF(K16=0,0,IFERROR(K16/M16,"Error"))</f>
+        <v>2.4691358024691357E-2</v>
+      </c>
+      <c r="F26" s="75"/>
       <c r="G26" s="36"/>
       <c r="H26" s="37"/>
       <c r="I26" s="37"/>
@@ -2051,16 +2074,19 @@
       <c r="N26" s="39"/>
     </row>
     <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="56" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="57"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="54">
-        <f>IF(K17=0,0,IFERROR(K17/M17,"Error"))</f>
-        <v>0</v>
-      </c>
-      <c r="F27" s="55"/>
+      <c r="B27" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="59"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="43">
+        <f>E4</f>
+        <v>3.4722222222222654E-3</v>
+      </c>
+      <c r="F27" s="44">
+        <f t="shared" ref="F27:F31" si="3">IF(E27="Completar",E27,IFERROR(E27/$E$32,"Error"))</f>
+        <v>2.3041474654378162E-2</v>
+      </c>
       <c r="G27" s="36"/>
       <c r="H27" s="37"/>
       <c r="I27" s="37"/>
@@ -2071,18 +2097,18 @@
       <c r="N27" s="39"/>
     </row>
     <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="56" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="57"/>
-      <c r="D28" s="58"/>
+      <c r="B28" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="59"/>
+      <c r="D28" s="60"/>
       <c r="E28" s="43">
-        <f>E4</f>
-        <v>3.4722222222222654E-3</v>
-      </c>
-      <c r="F28" s="44" t="str">
-        <f t="shared" ref="F28:F32" si="3">IF(E28="Completar",E28,IFERROR(E28/$E$33,"Error"))</f>
-        <v>Error</v>
+        <f>E8</f>
+        <v>4.7916666666666607E-2</v>
+      </c>
+      <c r="F28" s="44">
+        <f t="shared" si="3"/>
+        <v>0.31797235023041431</v>
       </c>
       <c r="G28" s="36"/>
       <c r="H28" s="37"/>
@@ -2094,18 +2120,18 @@
       <c r="N28" s="39"/>
     </row>
     <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="56" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="57"/>
-      <c r="D29" s="58"/>
+      <c r="B29" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="59"/>
+      <c r="D29" s="60"/>
       <c r="E29" s="43">
-        <f>E8</f>
-        <v>4.7916666666666607E-2</v>
-      </c>
-      <c r="F29" s="44" t="str">
-        <f t="shared" si="3"/>
-        <v>Error</v>
+        <f>E20</f>
+        <v>5.2083333333333315E-2</v>
+      </c>
+      <c r="F29" s="44">
+        <f>IF(E29="Completar",E29,IFERROR(E29/$E$32,"Error"))</f>
+        <v>0.34562211981566804</v>
       </c>
       <c r="G29" s="36"/>
       <c r="H29" s="37"/>
@@ -2117,18 +2143,18 @@
       <c r="N29" s="39"/>
     </row>
     <row r="30" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="56" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="57"/>
-      <c r="D30" s="58"/>
+      <c r="B30" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="59"/>
+      <c r="D30" s="60"/>
       <c r="E30" s="43">
-        <f>E21</f>
-        <v>5.2083333333333315E-2</v>
-      </c>
-      <c r="F30" s="44" t="str">
-        <f>IF(E30="Completar",E30,IFERROR(E30/$E$33,"Error"))</f>
-        <v>Error</v>
+        <f>L16</f>
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="F30" s="44">
+        <f t="shared" si="3"/>
+        <v>1.8433179723502304E-2</v>
       </c>
       <c r="G30" s="36"/>
       <c r="H30" s="37"/>
@@ -2140,18 +2166,18 @@
       <c r="N30" s="39"/>
     </row>
     <row r="31" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="56" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="57"/>
-      <c r="D31" s="58"/>
+      <c r="B31" s="58" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="59"/>
+      <c r="D31" s="60"/>
       <c r="E31" s="43">
-        <f>L17</f>
-        <v>0</v>
-      </c>
-      <c r="F31" s="44" t="str">
+        <f>J16</f>
+        <v>4.4444444444444509E-2</v>
+      </c>
+      <c r="F31" s="44">
         <f t="shared" si="3"/>
-        <v>Error</v>
+        <v>0.29493087557603725</v>
       </c>
       <c r="G31" s="36"/>
       <c r="H31" s="37"/>
@@ -2162,53 +2188,31 @@
       <c r="M31" s="37"/>
       <c r="N31" s="39"/>
     </row>
-    <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" s="57"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="43" t="str">
-        <f>J17</f>
-        <v>Error</v>
-      </c>
-      <c r="F32" s="44" t="str">
-        <f t="shared" si="3"/>
-        <v>Error</v>
-      </c>
-      <c r="G32" s="36"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="37"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="37"/>
-      <c r="L32" s="37"/>
-      <c r="M32" s="37"/>
-      <c r="N32" s="39"/>
-    </row>
-    <row r="33" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="66" t="s">
+    <row r="32" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="67"/>
-      <c r="D33" s="68"/>
-      <c r="E33" s="59" t="str">
-        <f>IF(COUNTIF(E28:E32,"Error")=0,SUM(E28:E32),"Error")</f>
-        <v>Error</v>
-      </c>
-      <c r="F33" s="60"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="41"/>
-      <c r="J33" s="41"/>
-      <c r="K33" s="41"/>
-      <c r="L33" s="41"/>
-      <c r="M33" s="41"/>
-      <c r="N33" s="42"/>
-    </row>
-    <row r="34" spans="1:15" s="10" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
-      <c r="O34" s="16"/>
-    </row>
+      <c r="C32" s="80"/>
+      <c r="D32" s="81"/>
+      <c r="E32" s="76">
+        <f>IF(COUNTIF(E27:E31,"Error")=0,SUM(E27:E31),"Error")</f>
+        <v>0.15069444444444446</v>
+      </c>
+      <c r="F32" s="77"/>
+      <c r="G32" s="40"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="41"/>
+      <c r="K32" s="41"/>
+      <c r="L32" s="41"/>
+      <c r="M32" s="41"/>
+      <c r="N32" s="42"/>
+    </row>
+    <row r="33" spans="1:15" s="10" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="16"/>
+      <c r="O33" s="16"/>
+    </row>
+    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.25"/>
@@ -2232,15 +2236,36 @@
     <row r="55" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="56" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="57" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="58" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="58" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <mergeCells count="37">
+  <mergeCells count="36">
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="B22:N22"/>
+    <mergeCell ref="F4:N4"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="C11:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
     <mergeCell ref="C1:N1"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B23:D23"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="M11:M12"/>
     <mergeCell ref="N11:N12"/>
@@ -2249,30 +2274,8 @@
     <mergeCell ref="B10:N10"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B16:E16"/>
     <mergeCell ref="F3:N3"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="C11:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="B23:N23"/>
-    <mergeCell ref="F4:N4"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="H11:J11"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:XFD1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">

</xml_diff>